<commit_message>
looks like the bird is now moving left-to right. Possible issues with wraparound.
</commit_message>
<xml_diff>
--- a/bak/c64memmap.xlsx
+++ b/bak/c64memmap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lewisb/Documents/c64projects/swabdeck-c64/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57D3950F-B296-644D-B865-95DB9B7CE69C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E13C42-1057-A34D-BAED-6DACE837586D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-21100" windowWidth="28040" windowHeight="18220" xr2:uid="{F4CB558A-42F0-5F4F-836F-7B34C4BF3EB3}"/>
+    <workbookView xWindow="-15560" yWindow="-19840" windowWidth="28040" windowHeight="18220" xr2:uid="{F4CB558A-42F0-5F4F-836F-7B34C4BF3EB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Description</t>
   </si>
@@ -84,6 +84,21 @@
   </si>
   <si>
     <t>completely in VIC bank?</t>
+  </si>
+  <si>
+    <t>CHARDATA</t>
+  </si>
+  <si>
+    <t>_screen_data</t>
+  </si>
+  <si>
+    <t>_color_data</t>
+  </si>
+  <si>
+    <t>sprite data</t>
+  </si>
+  <si>
+    <t>ASM (entry)</t>
   </si>
 </sst>
 </file>
@@ -133,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -143,6 +158,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FE97D0-BF64-A541-B1FB-27E88E5C3C65}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:C19"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,15 +546,15 @@
         <f>_xlfn.CONCAT("$",DEC2HEX(E2,4))</f>
         <v>$0001</v>
       </c>
-      <c r="G2" s="2" t="str">
+      <c r="G2" s="5" t="str">
         <f>IF(E2&gt;=B3,"yes","no")</f>
         <v>no</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="5">
         <f>IF(B2&lt;=16383,0,IF(B2&lt;=32767,1,IF(B2&lt;=49151,2,3)))</f>
         <v>0</v>
       </c>
-      <c r="I2" s="2" t="str">
+      <c r="I2" s="5" t="str">
         <f>IF((B2+D2-1) &lt; ((H2+1)*16384),"yes", "no")</f>
         <v>yes</v>
       </c>
@@ -558,15 +581,15 @@
         <f>_xlfn.CONCAT("$",DEC2HEX(E3,4))</f>
         <v>$0002</v>
       </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G10" si="0">IF(E3&gt;=B4,"yes","no")</f>
-        <v>no</v>
-      </c>
-      <c r="H3">
+      <c r="G3" s="5" t="str">
+        <f t="shared" ref="G3:G14" si="0">IF(E3&gt;=B4,"yes","no")</f>
+        <v>no</v>
+      </c>
+      <c r="H3" s="5">
         <f t="shared" ref="H3:H10" si="1">IF(B3&lt;=16383,0,IF(B3&lt;=32767,1,IF(B3&lt;=49151,2,3)))</f>
         <v>0</v>
       </c>
-      <c r="I3" t="str">
+      <c r="I3" s="5" t="str">
         <f t="shared" ref="I3:I10" si="2">IF((B3+D3-1) &lt; ((H3+1)*16384),"yes", "no")</f>
         <v>yes</v>
       </c>
@@ -593,15 +616,15 @@
         <f>_xlfn.CONCAT("$",DEC2HEX(E4,4))</f>
         <v>$00FA</v>
       </c>
-      <c r="G4" s="2" t="str">
+      <c r="G4" s="5" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I4" s="2" t="str">
+      <c r="I4" s="5" t="str">
         <f t="shared" si="2"/>
         <v>yes</v>
       </c>
@@ -628,15 +651,15 @@
         <f>_xlfn.CONCAT("$",DEC2HEX(E5,4))</f>
         <v>$00FE</v>
       </c>
-      <c r="G5" t="str">
+      <c r="G5" s="5" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I5" t="str">
+      <c r="I5" s="5" t="str">
         <f t="shared" si="2"/>
         <v>yes</v>
       </c>
@@ -663,15 +686,15 @@
         <f>_xlfn.CONCAT("$",DEC2HEX(E6,4))</f>
         <v>$00FF</v>
       </c>
-      <c r="G6" s="2" t="str">
+      <c r="G6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I6" s="2" t="str">
+      <c r="I6" s="5" t="str">
         <f t="shared" si="2"/>
         <v>yes</v>
       </c>
@@ -698,15 +721,15 @@
         <f>_xlfn.CONCAT("$",DEC2HEX(E7,4))</f>
         <v>$03FF</v>
       </c>
-      <c r="G7" s="2" t="str">
+      <c r="G7" s="5" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I7" s="2" t="str">
+      <c r="I7" s="5" t="str">
         <f t="shared" si="2"/>
         <v>yes</v>
       </c>
@@ -733,89 +756,268 @@
         <f>_xlfn.CONCAT("$",DEC2HEX(E8,4))</f>
         <v>$07FF</v>
       </c>
-      <c r="G8" t="str">
+      <c r="G8" s="5" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I8" t="str">
+      <c r="I8" s="5" t="str">
         <f t="shared" si="2"/>
         <v>yes</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2049</v>
+      </c>
+      <c r="C9" s="8" t="str">
+        <f>_xlfn.CONCAT("$", DEC2HEX(B9,4))</f>
+        <v>$0801</v>
+      </c>
+      <c r="D9" s="4">
+        <v>258</v>
+      </c>
+      <c r="E9" s="7">
+        <f>B9+D9-1</f>
+        <v>2306</v>
+      </c>
+      <c r="F9" s="8" t="str">
+        <f>_xlfn.CONCAT("$",DEC2HEX(E9,4))</f>
+        <v>$0902</v>
+      </c>
+      <c r="G9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>no</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="5">
+        <v>11904</v>
+      </c>
+      <c r="C10" s="6" t="str">
+        <f>_xlfn.CONCAT("$", DEC2HEX(B10,4))</f>
+        <v>$2E80</v>
+      </c>
+      <c r="D10">
+        <f>6*64</f>
+        <v>384</v>
+      </c>
+      <c r="E10" s="5">
+        <f>B10+D10-1</f>
+        <v>12287</v>
+      </c>
+      <c r="F10" s="6" t="str">
+        <f>_xlfn.CONCAT("$",DEC2HEX(E10,4))</f>
+        <v>$2FFF</v>
+      </c>
+      <c r="G10" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>no</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5">
+        <v>12288</v>
+      </c>
+      <c r="C11" s="6" t="str">
+        <f>_xlfn.CONCAT("$", DEC2HEX(B11,4))</f>
+        <v>$3000</v>
+      </c>
+      <c r="D11" s="5">
+        <v>128</v>
+      </c>
+      <c r="E11" s="5">
+        <f>B11+D11-1</f>
+        <v>12415</v>
+      </c>
+      <c r="F11" s="6" t="str">
+        <f>_xlfn.CONCAT("$",DEC2HEX(E11,4))</f>
+        <v>$307F</v>
+      </c>
+      <c r="G11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>no</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" ref="H11:H15" si="3">IF(B11&lt;=16383,0,IF(B11&lt;=32767,1,IF(B11&lt;=49151,2,3)))</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="5" t="str">
+        <f t="shared" ref="I11:I14" si="4">IF((B11+D11-1) &lt; ((H11+1)*16384),"yes", "no")</f>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="5">
+        <v>38912</v>
+      </c>
+      <c r="C12" s="6" t="str">
+        <f>_xlfn.CONCAT("$", DEC2HEX(B12,4))</f>
+        <v>$9800</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1024</v>
+      </c>
+      <c r="E12" s="5">
+        <f>B12+D12-1</f>
+        <v>39935</v>
+      </c>
+      <c r="F12" s="6" t="str">
+        <f>_xlfn.CONCAT("$",DEC2HEX(E12,4))</f>
+        <v>$9BFF</v>
+      </c>
+      <c r="G12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>no</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I12" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="5">
+        <v>39936</v>
+      </c>
+      <c r="C13" s="6" t="str">
+        <f>_xlfn.CONCAT("$", DEC2HEX(B13,4))</f>
+        <v>$9C00</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1024</v>
+      </c>
+      <c r="E13" s="5">
+        <f>B13+D13-1</f>
+        <v>40959</v>
+      </c>
+      <c r="F13" s="6" t="str">
+        <f>_xlfn.CONCAT("$",DEC2HEX(E13,4))</f>
+        <v>$9FFF</v>
+      </c>
+      <c r="G13" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>no</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I13" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B14" s="2">
         <v>40960</v>
       </c>
-      <c r="C9" s="3" t="str">
-        <f>_xlfn.CONCAT("$", DEC2HEX(B9,4))</f>
+      <c r="C14" s="3" t="str">
+        <f>_xlfn.CONCAT("$", DEC2HEX(B14,4))</f>
         <v>$A000</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D14" s="2">
         <v>8192</v>
       </c>
-      <c r="E9" s="2">
-        <f>B9+D9-1</f>
+      <c r="E14" s="2">
+        <f>B14+D14-1</f>
         <v>49151</v>
       </c>
-      <c r="F9" s="3" t="str">
-        <f>_xlfn.CONCAT("$",DEC2HEX(E9,4))</f>
+      <c r="F14" s="3" t="str">
+        <f>_xlfn.CONCAT("$",DEC2HEX(E14,4))</f>
         <v>$BFFF</v>
       </c>
-      <c r="G9" s="2" t="str">
+      <c r="G14" s="5" t="str">
         <f t="shared" si="0"/>
         <v>no</v>
       </c>
-      <c r="H9" s="2">
-        <f t="shared" si="1"/>
+      <c r="H14" s="5">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="I9" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>yes</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="I14" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B15" s="2">
         <v>53248</v>
       </c>
-      <c r="C10" s="3" t="str">
-        <f>_xlfn.CONCAT("$", DEC2HEX(B10,4))</f>
+      <c r="C15" s="3" t="str">
+        <f>_xlfn.CONCAT("$", DEC2HEX(B15,4))</f>
         <v>$D000</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D15" s="2">
         <v>4096</v>
       </c>
-      <c r="E10" s="2">
-        <f>B10+D10-1</f>
+      <c r="E15" s="2">
+        <f>B15+D15-1</f>
         <v>57343</v>
       </c>
-      <c r="F10" s="3" t="str">
-        <f>_xlfn.CONCAT("$",DEC2HEX(E10,4))</f>
+      <c r="F15" s="3" t="str">
+        <f>_xlfn.CONCAT("$",DEC2HEX(E15,4))</f>
         <v>$DFFF</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2">
-        <f t="shared" si="1"/>
+      <c r="G15" s="5" t="str">
+        <f t="shared" ref="G15" si="5">IF(E15&gt;=B16,"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" ref="H15" si="6">IF(B15&lt;=16383,0,IF(B15&lt;=32767,1,IF(B15&lt;=49151,2,3)))</f>
         <v>3</v>
       </c>
-      <c r="I10" s="2" t="str">
-        <f t="shared" si="2"/>
+      <c r="I15" s="5" t="str">
+        <f t="shared" ref="I15" si="7">IF((B15+D15-1) &lt; ((H15+1)*16384),"yes", "no")</f>
         <v>yes</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F10">
-    <sortCondition ref="B2:B10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F15">
+    <sortCondition ref="B2:B15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>